<commit_message>
created generic plotting scripts in the scripts folder
</commit_message>
<xml_diff>
--- a/data/dose_response/THPa4_selectivity.xlsx
+++ b/data/dose_response/THPa4_selectivity.xlsx
@@ -13,11 +13,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Ligand concentration</t>
   </si>
   <si>
+    <t>Norlaudanosoline-1</t>
+  </si>
+  <si>
+    <t>Norlaudanosoline-2</t>
+  </si>
+  <si>
+    <t>Norlaudanosoline-3</t>
+  </si>
+  <si>
+    <t>Norreticuline_1</t>
+  </si>
+  <si>
+    <t>Norreticuline_2</t>
+  </si>
+  <si>
+    <t>Norreticuline_3</t>
+  </si>
+  <si>
+    <t>Tetrahydropapaverine_1</t>
+  </si>
+  <si>
+    <t>Tetrahydropapaverine_2</t>
+  </si>
+  <si>
+    <t>Tetrahydropapaverine_3</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
     <t>NOR_1</t>
   </si>
   <si>
@@ -43,9 +73,6 @@
   </si>
   <si>
     <t>THP_3</t>
-  </si>
-  <si>
-    <t>REFERENCE</t>
   </si>
   <si>
     <t>Title</t>
@@ -733,31 +760,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
@@ -1083,49 +1110,49 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="D3" s="7" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="D4" s="7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>